<commit_message>
Added a Date Column
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{31E8BEF3-8394-47B5-9A05-B367D404BBE1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C04768A9-3294-405D-BD78-D79EBE35B985}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="12240" windowHeight="8010" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>URL</t>
   </si>
@@ -87,6 +87,12 @@
   </si>
   <si>
     <t>Padhi</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>current date</t>
   </si>
 </sst>
 </file>
@@ -132,7 +138,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -155,18 +161,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -588,10 +607,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,9 +620,10 @@
     <col min="5" max="5" width="13.28515625" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
     <col min="7" max="7" width="29.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
@@ -625,8 +645,11 @@
       <c r="G1" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="H1" s="6" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -647,6 +670,9 @@
       </c>
       <c r="G2" s="5" t="s">
         <v>18</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>